<commit_message>
minor edits to MetricSources.xlsx
</commit_message>
<xml_diff>
--- a/data/prepped/MetricSources.xlsx
+++ b/data/prepped/MetricSources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seek/Documents/GitProjects/MyProjects/QRFcapacity/data/prepped/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\QRFcapacity\data\prepped\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C67A6DB-82B2-C342-815E-FFF47B3BC284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041946E-7B89-4A16-95D0-981942FD1DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5800" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{63395C09-D57F-C64C-B6BC-1B1F1C19F834}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{63395C09-D57F-C64C-B6BC-1B1F1C19F834}"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -660,7 +660,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -698,12 +698,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -776,19 +770,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -818,31 +806,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color theme="4" tint="-0.499984740745262"/>
@@ -850,16 +824,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1273,109 +1237,109 @@
   <dimension ref="A1:R123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N97" sqref="N97"/>
+      <selection pane="bottomRight" activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" customWidth="1"/>
-    <col min="12" max="12" width="33.83203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.69921875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.19921875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.69921875" customWidth="1"/>
+    <col min="10" max="10" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.796875" customWidth="1"/>
+    <col min="12" max="12" width="33.796875" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="27.5" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="H1" s="6" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="H1" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-    </row>
-    <row r="2" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>117</v>
       </c>
@@ -1385,13 +1349,13 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -1425,7 +1389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>118</v>
       </c>
@@ -1435,13 +1399,13 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1475,7 +1439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1485,13 +1449,13 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1525,7 +1489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>9</v>
       </c>
@@ -1535,13 +1499,13 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1569,7 +1533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>8</v>
       </c>
@@ -1579,13 +1543,13 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1613,7 +1577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -1623,16 +1587,16 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1660,7 +1624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1670,16 +1634,16 @@
       <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1713,7 +1677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>112</v>
       </c>
@@ -1723,13 +1687,13 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1763,7 +1727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>114</v>
       </c>
@@ -1773,13 +1737,13 @@
       <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1813,7 +1777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>116</v>
       </c>
@@ -1823,13 +1787,13 @@
       <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1863,7 +1827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>115</v>
       </c>
@@ -1873,13 +1837,13 @@
       <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="D13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1913,7 +1877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>113</v>
       </c>
@@ -1923,13 +1887,13 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="D14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1963,7 +1927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>111</v>
       </c>
@@ -1973,13 +1937,13 @@
       <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="E15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -2013,7 +1977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -2023,13 +1987,13 @@
       <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="E16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2063,7 +2027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>23</v>
       </c>
@@ -2073,13 +2037,13 @@
       <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="E17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -2113,7 +2077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>58</v>
       </c>
@@ -2123,13 +2087,13 @@
       <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="E18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -2163,7 +2127,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>25</v>
       </c>
@@ -2173,13 +2137,13 @@
       <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="E19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -2213,7 +2177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>24</v>
       </c>
@@ -2223,13 +2187,13 @@
       <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="7" t="s">
+      <c r="E20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -2263,7 +2227,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2273,13 +2237,13 @@
       <c r="C21" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="E21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -2313,7 +2277,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -2323,13 +2287,13 @@
       <c r="C22" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="7" t="s">
+      <c r="E22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2363,7 +2327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>57</v>
       </c>
@@ -2373,13 +2337,13 @@
       <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="E23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -2413,7 +2377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -2423,13 +2387,13 @@
       <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="E24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -2463,7 +2427,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>20</v>
       </c>
@@ -2473,13 +2437,13 @@
       <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="7" t="s">
+      <c r="E25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -2513,7 +2477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -2523,13 +2487,13 @@
       <c r="C26" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="7" t="s">
+      <c r="E26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2563,7 +2527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -2573,13 +2537,13 @@
       <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="E27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2613,7 +2577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>56</v>
       </c>
@@ -2623,13 +2587,13 @@
       <c r="C28" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="7" t="s">
+      <c r="E28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2663,7 +2627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>17</v>
       </c>
@@ -2673,13 +2637,13 @@
       <c r="C29" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="7" t="s">
+      <c r="E29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2713,7 +2677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>16</v>
       </c>
@@ -2723,13 +2687,13 @@
       <c r="C30" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="7" t="s">
+      <c r="E30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2763,7 +2727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>42</v>
       </c>
@@ -2773,13 +2737,13 @@
       <c r="C31" t="s">
         <v>51</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="7" t="s">
+      <c r="E31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2813,7 +2777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>40</v>
       </c>
@@ -2823,13 +2787,13 @@
       <c r="C32" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="7" t="s">
+      <c r="E32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -2863,7 +2827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>47</v>
       </c>
@@ -2873,13 +2837,13 @@
       <c r="C33" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="7" t="s">
+      <c r="E33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -2913,7 +2877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>46</v>
       </c>
@@ -2923,13 +2887,13 @@
       <c r="C34" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="7" t="s">
+      <c r="E34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -2963,7 +2927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44</v>
       </c>
@@ -2973,13 +2937,13 @@
       <c r="C35" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="7" t="s">
+      <c r="E35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H35" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -3013,7 +2977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -3023,16 +2987,16 @@
       <c r="C36" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="7" t="s">
+      <c r="E36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H36" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -3066,7 +3030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3076,16 +3040,16 @@
       <c r="C37" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="7" t="s">
+      <c r="D37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -3113,7 +3077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>43</v>
       </c>
@@ -3123,16 +3087,16 @@
       <c r="C38" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="7" t="s">
+      <c r="D38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -3166,7 +3130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>27</v>
       </c>
@@ -3176,13 +3140,13 @@
       <c r="C39" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="7" t="s">
+      <c r="E39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -3216,7 +3180,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>41</v>
       </c>
@@ -3226,13 +3190,13 @@
       <c r="C40" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="7" t="s">
+      <c r="E40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="H40" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I40" s="1" t="s">
@@ -3260,7 +3224,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -3270,13 +3234,13 @@
       <c r="C41" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="7" t="s">
+      <c r="E41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H41" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -3310,7 +3274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>51</v>
       </c>
@@ -3320,16 +3284,16 @@
       <c r="C42" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="7" t="s">
+      <c r="D42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -3363,7 +3327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>50</v>
       </c>
@@ -3373,16 +3337,16 @@
       <c r="C43" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" s="7" t="s">
+      <c r="D43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H43" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -3416,7 +3380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>48</v>
       </c>
@@ -3426,16 +3390,16 @@
       <c r="C44" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="7" t="s">
+      <c r="D44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -3469,7 +3433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>103</v>
       </c>
@@ -3479,16 +3443,16 @@
       <c r="C45" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="7" t="s">
+      <c r="D45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -3522,7 +3486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>100</v>
       </c>
@@ -3532,16 +3496,16 @@
       <c r="C46" t="s">
         <v>70</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="7" t="s">
+      <c r="D46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="H46" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -3575,7 +3539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>96</v>
       </c>
@@ -3585,16 +3549,16 @@
       <c r="C47" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="7" t="s">
+      <c r="D47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="H47" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3628,7 +3592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>101</v>
       </c>
@@ -3638,16 +3602,16 @@
       <c r="C48" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="7" t="s">
+      <c r="D48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="H48" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -3681,7 +3645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>106</v>
       </c>
@@ -3691,16 +3655,16 @@
       <c r="C49" t="s">
         <v>73</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="7" t="s">
+      <c r="D49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H49" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -3734,7 +3698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>99</v>
       </c>
@@ -3744,16 +3708,16 @@
       <c r="C50" t="s">
         <v>74</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="7" t="s">
+      <c r="D50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="H50" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -3787,7 +3751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>91</v>
       </c>
@@ -3797,16 +3761,16 @@
       <c r="C51" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="7" t="s">
+      <c r="D51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -3840,7 +3804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>108</v>
       </c>
@@ -3850,13 +3814,13 @@
       <c r="C52" t="s">
         <v>76</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="7" t="s">
+      <c r="E52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -3890,7 +3854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>107</v>
       </c>
@@ -3900,13 +3864,13 @@
       <c r="C53" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="7" t="s">
+      <c r="E53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H53" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -3940,7 +3904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>10</v>
       </c>
@@ -3950,13 +3914,13 @@
       <c r="C54" t="s">
         <v>78</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="7" t="s">
+      <c r="F54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -3990,7 +3954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>11</v>
       </c>
@@ -4000,13 +3964,13 @@
       <c r="C55" t="s">
         <v>80</v>
       </c>
-      <c r="F55" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="7" t="s">
+      <c r="F55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H55" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -4034,7 +3998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>12</v>
       </c>
@@ -4044,13 +4008,13 @@
       <c r="C56" t="s">
         <v>81</v>
       </c>
-      <c r="F56" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="7" t="s">
+      <c r="F56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -4078,7 +4042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>6</v>
       </c>
@@ -4088,19 +4052,19 @@
       <c r="C57" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="7" t="s">
+      <c r="D57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H57" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -4128,7 +4092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>77</v>
       </c>
@@ -4138,16 +4102,16 @@
       <c r="C58" t="s">
         <v>83</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="7" t="s">
+      <c r="D58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H58" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I58" s="1" t="s">
@@ -4181,7 +4145,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>90</v>
       </c>
@@ -4191,19 +4155,19 @@
       <c r="C59" t="s">
         <v>85</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="7" t="s">
+      <c r="D59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H59" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -4237,7 +4201,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>78</v>
       </c>
@@ -4247,16 +4211,16 @@
       <c r="C60" t="s">
         <v>86</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="7" t="s">
+      <c r="D60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H60" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -4290,7 +4254,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>79</v>
       </c>
@@ -4300,16 +4264,16 @@
       <c r="C61" t="s">
         <v>87</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="7" t="s">
+      <c r="D61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -4343,7 +4307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>94</v>
       </c>
@@ -4353,16 +4317,16 @@
       <c r="C62" t="s">
         <v>88</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="7" t="s">
+      <c r="D62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -4396,7 +4360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>80</v>
       </c>
@@ -4406,16 +4370,16 @@
       <c r="C63" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="7" t="s">
+      <c r="D63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H63" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I63" s="1" t="s">
@@ -4449,7 +4413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>81</v>
       </c>
@@ -4459,16 +4423,16 @@
       <c r="C64" t="s">
         <v>90</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="7" t="s">
+      <c r="D64" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I64" s="1" t="s">
@@ -4502,7 +4466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>93</v>
       </c>
@@ -4512,16 +4476,16 @@
       <c r="C65" t="s">
         <v>91</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="7" t="s">
+      <c r="D65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I65" s="1" t="s">
@@ -4555,7 +4519,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>82</v>
       </c>
@@ -4565,16 +4529,16 @@
       <c r="C66" t="s">
         <v>92</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="7" t="s">
+      <c r="D66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I66" s="1" t="s">
@@ -4608,17 +4572,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
         <v>159</v>
       </c>
-      <c r="E67" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="7" t="s">
+      <c r="E67" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H67" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I67" s="1" t="s">
@@ -4648,7 +4612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>54</v>
       </c>
@@ -4658,13 +4622,13 @@
       <c r="C68" t="s">
         <v>93</v>
       </c>
-      <c r="E68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="7" t="s">
+      <c r="E68" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I68" s="1" t="s">
@@ -4692,7 +4656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>109</v>
       </c>
@@ -4702,16 +4666,16 @@
       <c r="C69" t="s">
         <v>95</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="7" t="s">
+      <c r="D69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I69" s="1" t="s">
@@ -4745,7 +4709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>110</v>
       </c>
@@ -4755,13 +4719,13 @@
       <c r="C70" t="s">
         <v>96</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="7" t="s">
+      <c r="E70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I70" s="1" t="s">
@@ -4795,7 +4759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>62</v>
       </c>
@@ -4805,13 +4769,13 @@
       <c r="C71" t="s">
         <v>97</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="7" t="s">
+      <c r="E71" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H71" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I71" s="1" t="s">
@@ -4845,7 +4809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>65</v>
       </c>
@@ -4855,13 +4819,13 @@
       <c r="C72" t="s">
         <v>98</v>
       </c>
-      <c r="E72" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G72" s="7" t="s">
+      <c r="E72" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H72" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I72" s="1" t="s">
@@ -4895,7 +4859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>64</v>
       </c>
@@ -4905,13 +4869,13 @@
       <c r="C73" t="s">
         <v>99</v>
       </c>
-      <c r="E73" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="7" t="s">
+      <c r="E73" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H73" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I73" s="1" t="s">
@@ -4945,7 +4909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>66</v>
       </c>
@@ -4955,13 +4919,13 @@
       <c r="C74" t="s">
         <v>100</v>
       </c>
-      <c r="E74" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" s="7" t="s">
+      <c r="E74" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H74" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I74" s="1" t="s">
@@ -4995,7 +4959,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>63</v>
       </c>
@@ -5005,13 +4969,13 @@
       <c r="C75" t="s">
         <v>101</v>
       </c>
-      <c r="E75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="7" t="s">
+      <c r="E75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="H75" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I75" s="1" t="s">
@@ -5045,7 +5009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>61</v>
       </c>
@@ -5055,13 +5019,13 @@
       <c r="C76" t="s">
         <v>102</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G76" s="7" t="s">
+      <c r="E76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H76" s="5" t="s">
+      <c r="H76" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I76" s="1" t="s">
@@ -5095,7 +5059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>55</v>
       </c>
@@ -5105,16 +5069,16 @@
       <c r="C77" t="s">
         <v>103</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" s="7" t="s">
+      <c r="D77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H77" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I77" s="1" t="s">
@@ -5148,7 +5112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>7</v>
       </c>
@@ -5158,19 +5122,19 @@
       <c r="C78" t="s">
         <v>104</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" s="7" t="s">
+      <c r="D78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I78" s="1" t="s">
@@ -5204,7 +5168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>13</v>
       </c>
@@ -5214,13 +5178,13 @@
       <c r="C79" t="s">
         <v>106</v>
       </c>
-      <c r="E79" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="7" t="s">
+      <c r="E79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H79" s="5" t="s">
+      <c r="H79" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I79" s="1" t="s">
@@ -5248,7 +5212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>5</v>
       </c>
@@ -5258,16 +5222,16 @@
       <c r="C80" t="s">
         <v>107</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G80" s="7" t="s">
+      <c r="D80" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H80" s="5" t="s">
+      <c r="H80" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I80" s="1" t="s">
@@ -5295,7 +5259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>30</v>
       </c>
@@ -5305,16 +5269,16 @@
       <c r="C81" t="s">
         <v>108</v>
       </c>
-      <c r="D81" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" s="7" t="s">
+      <c r="D81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H81" s="5" t="s">
+      <c r="H81" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I81" s="1" t="s">
@@ -5348,7 +5312,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>29</v>
       </c>
@@ -5358,16 +5322,16 @@
       <c r="C82" t="s">
         <v>109</v>
       </c>
-      <c r="D82" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G82" s="7" t="s">
+      <c r="D82" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H82" s="5" t="s">
+      <c r="H82" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I82" s="1" t="s">
@@ -5401,7 +5365,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>36</v>
       </c>
@@ -5411,13 +5375,13 @@
       <c r="C83" t="s">
         <v>110</v>
       </c>
-      <c r="E83" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" s="7" t="s">
+      <c r="E83" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H83" s="5" t="s">
+      <c r="H83" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I83" s="1" t="s">
@@ -5451,7 +5415,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>45</v>
       </c>
@@ -5461,13 +5425,13 @@
       <c r="C84" t="s">
         <v>111</v>
       </c>
-      <c r="E84" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G84" s="7" t="s">
+      <c r="E84" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H84" s="5" t="s">
+      <c r="H84" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -5501,7 +5465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>34</v>
       </c>
@@ -5511,13 +5475,13 @@
       <c r="C85" t="s">
         <v>112</v>
       </c>
-      <c r="E85" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G85" s="7" t="s">
+      <c r="E85" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H85" s="5" t="s">
+      <c r="H85" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I85" s="2" t="s">
@@ -5545,7 +5509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>53</v>
       </c>
@@ -5555,13 +5519,13 @@
       <c r="C86" t="s">
         <v>113</v>
       </c>
-      <c r="E86" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G86" s="7" t="s">
+      <c r="E86" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H86" s="5" t="s">
+      <c r="H86" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I86" s="2" t="s">
@@ -5595,7 +5559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>52</v>
       </c>
@@ -5605,13 +5569,13 @@
       <c r="C87" t="s">
         <v>114</v>
       </c>
-      <c r="E87" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G87" s="7" t="s">
+      <c r="E87" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H87" s="5" t="s">
+      <c r="H87" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I87" s="2" t="s">
@@ -5645,7 +5609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>59</v>
       </c>
@@ -5655,16 +5619,16 @@
       <c r="C88" t="s">
         <v>115</v>
       </c>
-      <c r="D88" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G88" s="7" t="s">
+      <c r="D88" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H88" s="5" t="s">
+      <c r="H88" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I88" s="1" t="s">
@@ -5698,7 +5662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>26</v>
       </c>
@@ -5708,16 +5672,16 @@
       <c r="C89" t="s">
         <v>116</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E89" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="7" t="s">
+      <c r="E89" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H89" s="5" t="s">
+      <c r="H89" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I89" s="1" t="s">
@@ -5751,7 +5715,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>39</v>
       </c>
@@ -5761,13 +5725,13 @@
       <c r="C90" t="s">
         <v>117</v>
       </c>
-      <c r="E90" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" s="7" t="s">
+      <c r="E90" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H90" s="5" t="s">
+      <c r="H90" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I90" s="1" t="s">
@@ -5801,7 +5765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>28</v>
       </c>
@@ -5811,19 +5775,19 @@
       <c r="C91" t="s">
         <v>118</v>
       </c>
-      <c r="D91" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G91" s="7" t="s">
+      <c r="D91" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H91" s="5" t="s">
+      <c r="H91" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I91" s="1" t="s">
@@ -5857,7 +5821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>37</v>
       </c>
@@ -5867,16 +5831,16 @@
       <c r="C92" t="s">
         <v>119</v>
       </c>
-      <c r="D92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G92" s="7" t="s">
+      <c r="D92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H92" s="5" t="s">
+      <c r="H92" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I92" s="1" t="s">
@@ -5910,7 +5874,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>60</v>
       </c>
@@ -5920,16 +5884,16 @@
       <c r="C93" t="s">
         <v>120</v>
       </c>
-      <c r="D93" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G93" s="7" t="s">
+      <c r="D93" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H93" s="5" t="s">
+      <c r="H93" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I93" s="1" t="s">
@@ -5963,7 +5927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>67</v>
       </c>
@@ -5973,13 +5937,13 @@
       <c r="C94" t="s">
         <v>121</v>
       </c>
-      <c r="E94" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G94" s="7" t="s">
+      <c r="E94" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H94" s="5" t="s">
+      <c r="H94" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I94" s="1" t="s">
@@ -6013,7 +5977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>31</v>
       </c>
@@ -6023,16 +5987,16 @@
       <c r="C95" t="s">
         <v>123</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G95" s="7" t="s">
+      <c r="D95" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H95" s="5" t="s">
+      <c r="H95" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I95" s="1" t="s">
@@ -6066,7 +6030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>49</v>
       </c>
@@ -6076,16 +6040,16 @@
       <c r="C96" t="s">
         <v>124</v>
       </c>
-      <c r="D96" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G96" s="7" t="s">
+      <c r="D96" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H96" s="5" t="s">
+      <c r="H96" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I96" s="1" t="s">
@@ -6119,7 +6083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>32</v>
       </c>
@@ -6129,16 +6093,16 @@
       <c r="C97" t="s">
         <v>125</v>
       </c>
-      <c r="D97" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G97" s="7" t="s">
+      <c r="D97" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H97" s="5" t="s">
+      <c r="H97" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I97" s="1" t="s">
@@ -6166,7 +6130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>70</v>
       </c>
@@ -6176,16 +6140,16 @@
       <c r="C98" t="s">
         <v>126</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G98" s="7" t="s">
+      <c r="D98" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H98" s="5" t="s">
+      <c r="H98" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I98" s="1" t="s">
@@ -6219,7 +6183,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>71</v>
       </c>
@@ -6229,16 +6193,16 @@
       <c r="C99" t="s">
         <v>128</v>
       </c>
-      <c r="D99" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G99" s="7" t="s">
+      <c r="D99" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H99" s="5" t="s">
+      <c r="H99" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I99" s="1" t="s">
@@ -6272,7 +6236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>72</v>
       </c>
@@ -6282,16 +6246,16 @@
       <c r="C100" t="s">
         <v>129</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G100" s="7" t="s">
+      <c r="D100" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H100" s="5" t="s">
+      <c r="H100" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I100" s="1" t="s">
@@ -6325,7 +6289,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>68</v>
       </c>
@@ -6335,16 +6299,16 @@
       <c r="C101" t="s">
         <v>130</v>
       </c>
-      <c r="D101" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G101" s="7" t="s">
+      <c r="D101" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H101" s="5" t="s">
+      <c r="H101" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I101" s="1" t="s">
@@ -6378,7 +6342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>69</v>
       </c>
@@ -6388,16 +6352,16 @@
       <c r="C102" t="s">
         <v>131</v>
       </c>
-      <c r="D102" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G102" s="7" t="s">
+      <c r="D102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H102" s="5" t="s">
+      <c r="H102" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I102" s="1" t="s">
@@ -6425,7 +6389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>104</v>
       </c>
@@ -6435,16 +6399,16 @@
       <c r="C103" t="s">
         <v>132</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G103" s="7" t="s">
+      <c r="D103" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H103" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I103" s="1" t="s">
@@ -6478,7 +6442,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>105</v>
       </c>
@@ -6488,16 +6452,16 @@
       <c r="C104" t="s">
         <v>133</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G104" s="7" t="s">
+      <c r="D104" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H104" s="5" t="s">
+      <c r="H104" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I104" s="1" t="s">
@@ -6531,7 +6495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>95</v>
       </c>
@@ -6541,16 +6505,16 @@
       <c r="C105" t="s">
         <v>134</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" s="7" t="s">
+      <c r="D105" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H105" s="5" t="s">
+      <c r="H105" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I105" s="1" t="s">
@@ -6584,7 +6548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>97</v>
       </c>
@@ -6594,16 +6558,16 @@
       <c r="C106" t="s">
         <v>135</v>
       </c>
-      <c r="D106" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G106" s="7" t="s">
+      <c r="D106" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H106" s="5" t="s">
+      <c r="H106" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I106" s="1" t="s">
@@ -6637,7 +6601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>73</v>
       </c>
@@ -6647,16 +6611,16 @@
       <c r="C107" t="s">
         <v>136</v>
       </c>
-      <c r="D107" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G107" s="7" t="s">
+      <c r="D107" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H107" s="5" t="s">
+      <c r="H107" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I107" s="1" t="s">
@@ -6684,7 +6648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>74</v>
       </c>
@@ -6694,16 +6658,16 @@
       <c r="C108" t="s">
         <v>137</v>
       </c>
-      <c r="D108" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E108" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G108" s="7" t="s">
+      <c r="D108" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H108" s="5" t="s">
+      <c r="H108" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I108" s="1" t="s">
@@ -6731,7 +6695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>1</v>
       </c>
@@ -6741,16 +6705,16 @@
       <c r="C109" t="s">
         <v>138</v>
       </c>
-      <c r="D109" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G109" s="7" t="s">
+      <c r="D109" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H109" s="5" t="s">
+      <c r="H109" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I109" s="1" t="s">
@@ -6784,7 +6748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>92</v>
       </c>
@@ -6794,16 +6758,16 @@
       <c r="C110" t="s">
         <v>140</v>
       </c>
-      <c r="E110" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G110" s="7" t="s">
+      <c r="E110" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H110" s="5" t="s">
+      <c r="H110" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I110" s="1" t="s">
@@ -6837,20 +6801,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
         <v>163</v>
       </c>
-      <c r="E111" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="7" t="s">
+      <c r="E111" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H111" s="5" t="s">
+      <c r="H111" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I111" s="1" t="s">
@@ -6884,7 +6848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>76</v>
       </c>
@@ -6894,13 +6858,13 @@
       <c r="C112" t="s">
         <v>141</v>
       </c>
-      <c r="E112" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="7" t="s">
+      <c r="E112" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H112" s="5" t="s">
+      <c r="H112" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I112" s="1" t="s">
@@ -6934,7 +6898,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>75</v>
       </c>
@@ -6944,13 +6908,13 @@
       <c r="C113" t="s">
         <v>143</v>
       </c>
-      <c r="E113" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G113" s="7" t="s">
+      <c r="E113" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H113" s="5" t="s">
+      <c r="H113" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I113" s="1" t="s">
@@ -6984,7 +6948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>89</v>
       </c>
@@ -6994,13 +6958,13 @@
       <c r="C114" t="s">
         <v>144</v>
       </c>
-      <c r="E114" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="7" t="s">
+      <c r="E114" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H114" s="5" t="s">
+      <c r="H114" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I114" s="1" t="s">
@@ -7034,7 +6998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>119</v>
       </c>
@@ -7044,17 +7008,17 @@
       <c r="C115" t="s">
         <v>145</v>
       </c>
-      <c r="D115" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G115" s="7" t="s">
+      <c r="D115" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H115" s="5" t="s">
+      <c r="H115" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="J115" s="1" t="s">
         <v>12</v>
@@ -7084,7 +7048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>102</v>
       </c>
@@ -7094,13 +7058,13 @@
       <c r="C116" t="s">
         <v>147</v>
       </c>
-      <c r="E116" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G116" s="7" t="s">
+      <c r="E116" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H116" s="5" t="s">
+      <c r="H116" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I116" s="1" t="s">
@@ -7134,7 +7098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>98</v>
       </c>
@@ -7144,17 +7108,17 @@
       <c r="C117" t="s">
         <v>148</v>
       </c>
-      <c r="E117" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G117" s="7" t="s">
+      <c r="E117" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H117" s="5" t="s">
+      <c r="H117" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="J117" s="1" t="s">
         <v>20</v>
@@ -7184,7 +7148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>84</v>
       </c>
@@ -7194,20 +7158,20 @@
       <c r="C118" t="s">
         <v>149</v>
       </c>
-      <c r="D118" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E118" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G118" s="7" t="s">
+      <c r="D118" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H118" s="5" t="s">
+      <c r="H118" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="J118" s="1" t="s">
         <v>20</v>
@@ -7237,7 +7201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>86</v>
       </c>
@@ -7247,13 +7211,13 @@
       <c r="C119" t="s">
         <v>150</v>
       </c>
-      <c r="E119" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G119" s="7" t="s">
+      <c r="E119" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H119" s="5" t="s">
+      <c r="H119" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I119" s="1" t="s">
@@ -7287,7 +7251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>83</v>
       </c>
@@ -7297,20 +7261,20 @@
       <c r="C120" t="s">
         <v>151</v>
       </c>
-      <c r="D120" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E120" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G120" s="7" t="s">
+      <c r="D120" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H120" s="5" t="s">
+      <c r="H120" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="J120" s="1" t="s">
         <v>12</v>
@@ -7340,7 +7304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>88</v>
       </c>
@@ -7350,13 +7314,13 @@
       <c r="C121" t="s">
         <v>152</v>
       </c>
-      <c r="E121" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G121" s="7" t="s">
+      <c r="E121" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G121" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H121" s="5" t="s">
+      <c r="H121" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I121" s="1" t="s">
@@ -7390,7 +7354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>87</v>
       </c>
@@ -7400,13 +7364,13 @@
       <c r="C122" t="s">
         <v>153</v>
       </c>
-      <c r="E122" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G122" s="7" t="s">
+      <c r="E122" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H122" s="5" t="s">
+      <c r="H122" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I122" s="1" t="s">
@@ -7440,7 +7404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>85</v>
       </c>
@@ -7450,13 +7414,13 @@
       <c r="C123" t="s">
         <v>154</v>
       </c>
-      <c r="E123" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G123" s="7" t="s">
+      <c r="E123" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G123" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H123" s="5" t="s">
+      <c r="H123" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I123" s="1" t="s">
@@ -7497,28 +7461,28 @@
     <mergeCell ref="H1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:K83 I88:K1048576 I111:P111 H1">
-    <cfRule type="endsWith" dxfId="8" priority="6" operator="endsWith" text="?">
+    <cfRule type="endsWith" dxfId="5" priority="6" operator="endsWith" text="?">
       <formula>RIGHT(H1,LEN("?"))="?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:R67 I78:R80 I68:Q77 I81:Q88 I89:R114 I124:R1048576 I115:Q123 H1">
-    <cfRule type="endsWith" dxfId="7" priority="5" operator="endsWith" text="?">
+    <cfRule type="endsWith" dxfId="4" priority="5" operator="endsWith" text="?">
       <formula>RIGHT(H1,LEN("?"))="?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="endsWith" dxfId="6" priority="4" operator="endsWith" text="?">
+    <cfRule type="endsWith" dxfId="3" priority="4" operator="endsWith" text="?">
       <formula>RIGHT(H1,LEN("?"))="?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:R1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Maybe"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>